<commit_message>
Completing the test data for the permission tests.
</commit_message>
<xml_diff>
--- a/selenium_tests/manage_people/test_data/roles_access.xlsx
+++ b/selenium_tests/manage_people/test_data/roles_access.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15260" yWindow="-22740" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
-    <sheet name="Roles mapping " sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Site Setup" sheetId="2" r:id="rId2"/>
+    <sheet name="Migrations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">denied_roles </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t xml:space="preserve">Roles </t>
   </si>
@@ -86,9 +83,6 @@
     <t>tlttest54@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Access to Emailer </t>
-  </si>
-  <si>
     <t xml:space="preserve">Course or Account Level Roles </t>
   </si>
   <si>
@@ -129,13 +123,46 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access to MANAGE PEOPLE </t>
+  </si>
+  <si>
+    <t>92241</t>
+  </si>
+  <si>
+    <t>92242</t>
+  </si>
+  <si>
+    <t>92229</t>
+  </si>
+  <si>
+    <t>92230</t>
+  </si>
+  <si>
+    <t>90670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92238 </t>
+  </si>
+  <si>
+    <t>92235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canvas_user_id </t>
+  </si>
+  <si>
+    <t>https://github.com/Harvard-University-iCommons/canvas_course_admin_tools/blob/develop/manage_people/migrations/0001_mp_initial.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Migrations File and Roles </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,6 +215,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +241,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="146">
+  <cellStyleXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -353,8 +388,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -364,8 +411,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="129" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="146">
+  <cellStyles count="158">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -446,6 +494,18 @@
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -840,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -853,26 +913,82 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -891,7 +1007,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -899,196 +1015,196 @@
     <col min="1" max="1" width="39.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="31" style="4" customWidth="1"/>
     <col min="3" max="3" width="18" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="47.33203125" style="4" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4">
         <v>92241</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4">
         <v>92242</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4">
         <v>92229</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4">
         <v>92230</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4">
         <v>92232</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4">
         <v>92295</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4">
         <v>90670</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="4">
-        <v>92234</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <v>92238</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4">
-        <v>92235</v>
+        <v>92234</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4">
-        <v>92238</v>
+        <v>92235</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1100,9 +1216,9 @@
     <hyperlink ref="B6" r:id="rId5"/>
     <hyperlink ref="B7" r:id="rId6"/>
     <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B11" r:id="rId8"/>
+    <hyperlink ref="B12" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1116,24 +1232,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="142" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
+      <c r="A1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
- Updated and added to existing manage people permissions tests - Added all the various roles that will be under test for the test course and cleaned up for a cleaner looking format.
</commit_message>
<xml_diff>
--- a/selenium_tests/manage_people/test_data/roles_access.xlsx
+++ b/selenium_tests/manage_people/test_data/roles_access.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hic048/projects/canvas_manage_course/selenium_tests/manage_people/test_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
     <sheet name="Site Setup" sheetId="2" r:id="rId2"/>
-    <sheet name="Migrations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="80">
   <si>
     <t xml:space="preserve">Roles </t>
   </si>
@@ -125,9 +129,6 @@
     <t>no</t>
   </si>
   <si>
-    <t xml:space="preserve">Access to MANAGE PEOPLE </t>
-  </si>
-  <si>
     <t>92241</t>
   </si>
   <si>
@@ -143,26 +144,135 @@
     <t>90670</t>
   </si>
   <si>
-    <t xml:space="preserve">92238 </t>
-  </si>
-  <si>
-    <t>92235</t>
-  </si>
-  <si>
     <t xml:space="preserve">canvas_user_id </t>
   </si>
   <si>
-    <t>https://github.com/Harvard-University-iCommons/canvas_course_admin_tools/blob/develop/manage_people/migrations/0001_mp_initial.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Migrations File and Roles </t>
+    <t>Department Admin</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Librarian </t>
+  </si>
+  <si>
+    <t>Helpdesk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Level role (sub-account 10) </t>
+  </si>
+  <si>
+    <t>test12@mcelroy.org</t>
+  </si>
+  <si>
+    <t>test13@mcelroy.org</t>
+  </si>
+  <si>
+    <t>test36@mcelroy.org</t>
+  </si>
+  <si>
+    <t>test35@mcelroy.org</t>
+  </si>
+  <si>
+    <t>test34@mcelroy.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student </t>
+  </si>
+  <si>
+    <t>test9@mcelroy.org</t>
+  </si>
+  <si>
+    <t>test10@mcelroy.org</t>
+  </si>
+  <si>
+    <t>Prospective Enrollee</t>
+  </si>
+  <si>
+    <t>Access to MANAGE PEOPLE  
+for COLGSAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Observer </t>
+  </si>
+  <si>
+    <t>test37@mcelroy.org</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>92239</t>
+  </si>
+  <si>
+    <t>90675</t>
+  </si>
+  <si>
+    <t>92258</t>
+  </si>
+  <si>
+    <t>92260</t>
+  </si>
+  <si>
+    <t>92261</t>
+  </si>
+  <si>
+    <t>92259</t>
+  </si>
+  <si>
+    <t>92236</t>
+  </si>
+  <si>
+    <t>92237</t>
+  </si>
+  <si>
+    <t>92238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roles </t>
+  </si>
+  <si>
+    <t>Course Head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course Support Staff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faculty </t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Admin </t>
+  </si>
+  <si>
+    <t>Librarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School Liaison </t>
+  </si>
+  <si>
+    <t>92295</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,14 +325,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -405,13 +507,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="129" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="129"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="158">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -575,6 +679,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -900,311 +1009,577 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="31" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18" style="4" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="39.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32" style="3" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>92241</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>92242</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>92229</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>92230</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="3">
+        <v>92239</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="3">
+        <v>90675</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3">
+        <v>92238</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C9" s="3">
         <v>92232</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3">
+        <v>92234</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3">
+        <v>92235</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3">
+        <v>92237</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3">
+        <v>92236</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3">
+        <v>92295</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4">
-        <v>92295</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3">
+        <v>90670</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4">
-        <v>90670</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="E16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="3">
+        <v>92258</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4">
-        <v>92238</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="4">
-        <v>92234</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="4">
-        <v>92235</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>24</v>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3">
+        <v>92260</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="3">
+        <v>92261</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="3">
+        <v>92259</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1213,52 +1588,22 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B11" r:id="rId8"/>
-    <hyperlink ref="B12" r:id="rId9"/>
-    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
+    <hyperlink ref="B16" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B8" r:id="rId10"/>
+    <hyperlink ref="B6" r:id="rId11"/>
+    <hyperlink ref="B7" r:id="rId12"/>
+    <hyperlink ref="B18" r:id="rId13"/>
+    <hyperlink ref="B20" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B13" r:id="rId16"/>
+    <hyperlink ref="B12" r:id="rId17"/>
+    <hyperlink ref="B19" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="142" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>